<commit_message>
Update Colors and Model Accuracies
</commit_message>
<xml_diff>
--- a/datasets/MigratoryModel/CombinedMigratoryModel_GuthrieZone_Path.xlsx
+++ b/datasets/MigratoryModel/CombinedMigratoryModel_GuthrieZone_Path.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby Ford\Desktop\BantuMigration\Github\datasets\MigratoryModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EC6ABE-42D3-4AE1-B185-29BCAB29D522}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C94B87B-82C4-4614-8C0B-5A1112DC79AC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{48220AAF-5FA7-46D3-8056-2130CE6EF7AB}"/>
   </bookViews>
@@ -211,9 +211,6 @@
     <t>F-M</t>
   </si>
   <si>
-    <t>Currie et al., 2015</t>
-  </si>
-  <si>
     <t>F-E</t>
   </si>
   <si>
@@ -287,6 +284,9 @@
   </si>
   <si>
     <t>Current Work - Y-Chromosomal (1,000 reps)</t>
+  </si>
+  <si>
+    <t>Currie et al., 2013</t>
   </si>
 </sst>
 </file>
@@ -640,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB7D369B-DF5B-472F-B73D-7CCA41A92755}">
   <dimension ref="A1:I291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="L212" sqref="L212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,7 +682,7 @@
         <v>41</v>
       </c>
       <c r="I1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -708,10 +708,10 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -737,10 +737,10 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -766,10 +766,10 @@
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -795,10 +795,10 @@
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -824,10 +824,10 @@
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -853,10 +853,10 @@
         <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -882,10 +882,10 @@
         <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -911,10 +911,10 @@
         <v>5</v>
       </c>
       <c r="H9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -940,10 +940,10 @@
         <v>9</v>
       </c>
       <c r="H10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -969,10 +969,10 @@
         <v>7</v>
       </c>
       <c r="H11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -998,10 +998,10 @@
         <v>7</v>
       </c>
       <c r="H12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1027,10 +1027,10 @@
         <v>8</v>
       </c>
       <c r="H13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1056,10 +1056,10 @@
         <v>8</v>
       </c>
       <c r="H14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1085,10 +1085,10 @@
         <v>3</v>
       </c>
       <c r="H15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1114,10 +1114,10 @@
         <v>3</v>
       </c>
       <c r="H16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1143,10 +1143,10 @@
         <v>6</v>
       </c>
       <c r="H17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1172,10 +1172,10 @@
         <v>6</v>
       </c>
       <c r="H18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1201,10 +1201,10 @@
         <v>7</v>
       </c>
       <c r="H19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1230,10 +1230,10 @@
         <v>7</v>
       </c>
       <c r="H20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1259,10 +1259,10 @@
         <v>6</v>
       </c>
       <c r="H21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1288,10 +1288,10 @@
         <v>6</v>
       </c>
       <c r="H22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1317,10 +1317,10 @@
         <v>6</v>
       </c>
       <c r="H23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1346,10 +1346,10 @@
         <v>7</v>
       </c>
       <c r="H24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1375,10 +1375,10 @@
         <v>7</v>
       </c>
       <c r="H25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1404,10 +1404,10 @@
         <v>7</v>
       </c>
       <c r="H26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1433,10 +1433,10 @@
         <v>8</v>
       </c>
       <c r="H27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1462,10 +1462,10 @@
         <v>8</v>
       </c>
       <c r="H28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1491,10 +1491,10 @@
         <v>9</v>
       </c>
       <c r="H29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1520,10 +1520,10 @@
         <v>8</v>
       </c>
       <c r="H30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1549,10 +1549,10 @@
         <v>8</v>
       </c>
       <c r="H31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1578,10 +1578,10 @@
         <v>1</v>
       </c>
       <c r="H32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1607,10 +1607,10 @@
         <v>2</v>
       </c>
       <c r="H33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1636,10 +1636,10 @@
         <v>2</v>
       </c>
       <c r="H34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1665,10 +1665,10 @@
         <v>4</v>
       </c>
       <c r="H35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1694,10 +1694,10 @@
         <v>4</v>
       </c>
       <c r="H36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -1723,10 +1723,10 @@
         <v>5</v>
       </c>
       <c r="H37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1752,15 +1752,15 @@
         <v>5</v>
       </c>
       <c r="H38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -1781,10 +1781,10 @@
         <v>5</v>
       </c>
       <c r="H39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -1810,10 +1810,10 @@
         <v>9</v>
       </c>
       <c r="H40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -1839,10 +1839,10 @@
         <v>7</v>
       </c>
       <c r="H41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -1868,10 +1868,10 @@
         <v>7</v>
       </c>
       <c r="H42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -1897,10 +1897,10 @@
         <v>8</v>
       </c>
       <c r="H43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -1926,10 +1926,10 @@
         <v>8</v>
       </c>
       <c r="H44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -1955,10 +1955,10 @@
         <v>3</v>
       </c>
       <c r="H45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I45" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -1984,10 +1984,10 @@
         <v>3</v>
       </c>
       <c r="H46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -2013,10 +2013,10 @@
         <v>6</v>
       </c>
       <c r="H47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2042,15 +2042,15 @@
         <v>6</v>
       </c>
       <c r="H48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I48" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B49">
         <v>2</v>
@@ -2071,15 +2071,15 @@
         <v>6</v>
       </c>
       <c r="H49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -2100,15 +2100,15 @@
         <v>6</v>
       </c>
       <c r="H50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -2129,10 +2129,10 @@
         <v>7</v>
       </c>
       <c r="H51" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -2158,15 +2158,15 @@
         <v>6</v>
       </c>
       <c r="H52" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B53">
         <v>2</v>
@@ -2187,15 +2187,15 @@
         <v>7</v>
       </c>
       <c r="H53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I53" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -2216,10 +2216,10 @@
         <v>8</v>
       </c>
       <c r="H54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2245,10 +2245,10 @@
         <v>8</v>
       </c>
       <c r="H55" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2274,10 +2274,10 @@
         <v>8</v>
       </c>
       <c r="H56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2303,10 +2303,10 @@
         <v>9</v>
       </c>
       <c r="H57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I57" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -2332,10 +2332,10 @@
         <v>9</v>
       </c>
       <c r="H58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I58" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2361,10 +2361,10 @@
         <v>10</v>
       </c>
       <c r="H59" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2390,10 +2390,10 @@
         <v>7</v>
       </c>
       <c r="H60" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I60" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -2419,10 +2419,10 @@
         <v>9</v>
       </c>
       <c r="H61" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I61" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -2448,10 +2448,10 @@
         <v>1</v>
       </c>
       <c r="H62" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I62" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -2477,10 +2477,10 @@
         <v>2</v>
       </c>
       <c r="H63" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I63" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -2506,10 +2506,10 @@
         <v>2</v>
       </c>
       <c r="H64" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I64" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -2535,10 +2535,10 @@
         <v>4</v>
       </c>
       <c r="H65" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I65" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -2564,10 +2564,10 @@
         <v>4</v>
       </c>
       <c r="H66" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I66" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -2593,10 +2593,10 @@
         <v>5</v>
       </c>
       <c r="H67" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I67" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -2622,15 +2622,15 @@
         <v>5</v>
       </c>
       <c r="H68" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -2651,10 +2651,10 @@
         <v>5</v>
       </c>
       <c r="H69" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I69" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -2680,10 +2680,10 @@
         <v>9</v>
       </c>
       <c r="H70" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I70" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -2709,10 +2709,10 @@
         <v>7</v>
       </c>
       <c r="H71" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I71" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -2738,10 +2738,10 @@
         <v>7</v>
       </c>
       <c r="H72" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I72" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -2767,10 +2767,10 @@
         <v>8</v>
       </c>
       <c r="H73" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I73" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -2796,10 +2796,10 @@
         <v>8</v>
       </c>
       <c r="H74" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I74" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -2825,10 +2825,10 @@
         <v>3</v>
       </c>
       <c r="H75" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I75" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -2854,10 +2854,10 @@
         <v>3</v>
       </c>
       <c r="H76" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I76" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -2883,10 +2883,10 @@
         <v>6</v>
       </c>
       <c r="H77" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -2912,10 +2912,10 @@
         <v>6</v>
       </c>
       <c r="H78" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I78" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -2941,10 +2941,10 @@
         <v>8</v>
       </c>
       <c r="H79" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I79" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -2970,10 +2970,10 @@
         <v>8</v>
       </c>
       <c r="H80" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I80" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -2999,10 +2999,10 @@
         <v>7</v>
       </c>
       <c r="H81" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I81" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -3028,15 +3028,15 @@
         <v>7</v>
       </c>
       <c r="H82" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I82" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B83">
         <v>2</v>
@@ -3057,10 +3057,10 @@
         <v>6</v>
       </c>
       <c r="H83" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I83" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -3086,10 +3086,10 @@
         <v>6</v>
       </c>
       <c r="H84" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I84" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -3115,10 +3115,10 @@
         <v>6</v>
       </c>
       <c r="H85" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I85" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -3144,10 +3144,10 @@
         <v>6</v>
       </c>
       <c r="H86" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I86" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -3173,10 +3173,10 @@
         <v>7</v>
       </c>
       <c r="H87" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I87" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -3202,10 +3202,10 @@
         <v>7</v>
       </c>
       <c r="H88" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I88" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -3231,10 +3231,10 @@
         <v>8</v>
       </c>
       <c r="H89" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I89" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -3260,10 +3260,10 @@
         <v>9</v>
       </c>
       <c r="H90" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I90" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -3289,10 +3289,10 @@
         <v>7</v>
       </c>
       <c r="H91" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I91" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -3318,10 +3318,10 @@
         <v>1</v>
       </c>
       <c r="H92" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I92" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -3347,10 +3347,10 @@
         <v>2</v>
       </c>
       <c r="H93" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I93" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -3376,10 +3376,10 @@
         <v>2</v>
       </c>
       <c r="H94" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I94" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -3405,10 +3405,10 @@
         <v>4</v>
       </c>
       <c r="H95" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I95" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -3434,10 +3434,10 @@
         <v>4</v>
       </c>
       <c r="H96" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I96" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -3463,10 +3463,10 @@
         <v>5</v>
       </c>
       <c r="H97" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I97" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -3492,15 +3492,15 @@
         <v>5</v>
       </c>
       <c r="H98" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I98" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -3521,15 +3521,15 @@
         <v>5</v>
       </c>
       <c r="H99" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I99" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -3550,15 +3550,15 @@
         <v>8</v>
       </c>
       <c r="H100" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I100" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B101">
         <v>1</v>
@@ -3579,15 +3579,15 @@
         <v>7</v>
       </c>
       <c r="H101" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I101" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B102">
         <v>2</v>
@@ -3608,15 +3608,15 @@
         <v>7</v>
       </c>
       <c r="H102" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I102" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B103">
         <v>2</v>
@@ -3637,15 +3637,15 @@
         <v>9</v>
       </c>
       <c r="H103" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I103" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B104">
         <v>2</v>
@@ -3666,10 +3666,10 @@
         <v>8</v>
       </c>
       <c r="H104" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I104" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -3695,10 +3695,10 @@
         <v>3</v>
       </c>
       <c r="H105" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I105" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -3724,10 +3724,10 @@
         <v>3</v>
       </c>
       <c r="H106" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I106" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -3753,15 +3753,15 @@
         <v>6</v>
       </c>
       <c r="H107" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I107" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B108">
         <v>1</v>
@@ -3782,15 +3782,15 @@
         <v>6</v>
       </c>
       <c r="H108" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I108" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B109">
         <v>2</v>
@@ -3811,15 +3811,15 @@
         <v>6</v>
       </c>
       <c r="H109" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I109" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B110">
         <v>1</v>
@@ -3840,10 +3840,10 @@
         <v>6</v>
       </c>
       <c r="H110" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I110" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -3869,10 +3869,10 @@
         <v>6</v>
       </c>
       <c r="H111" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I111" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -3898,15 +3898,15 @@
         <v>8</v>
       </c>
       <c r="H112" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I112" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B113">
         <v>2</v>
@@ -3927,10 +3927,10 @@
         <v>7</v>
       </c>
       <c r="H113" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I113" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -3956,10 +3956,10 @@
         <v>7</v>
       </c>
       <c r="H114" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I114" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -3985,10 +3985,10 @@
         <v>7</v>
       </c>
       <c r="H115" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I115" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -4014,10 +4014,10 @@
         <v>7</v>
       </c>
       <c r="H116" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I116" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -4043,10 +4043,10 @@
         <v>8</v>
       </c>
       <c r="H117" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I117" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -4072,10 +4072,10 @@
         <v>8</v>
       </c>
       <c r="H118" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I118" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -4101,10 +4101,10 @@
         <v>9</v>
       </c>
       <c r="H119" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I119" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
@@ -4130,10 +4130,10 @@
         <v>7</v>
       </c>
       <c r="H120" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I120" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -4159,10 +4159,10 @@
         <v>8</v>
       </c>
       <c r="H121" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I121" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -4188,10 +4188,10 @@
         <v>1</v>
       </c>
       <c r="H122" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I122" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
@@ -4217,10 +4217,10 @@
         <v>2</v>
       </c>
       <c r="H123" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I123" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
@@ -4246,10 +4246,10 @@
         <v>2</v>
       </c>
       <c r="H124" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I124" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -4275,10 +4275,10 @@
         <v>3</v>
       </c>
       <c r="H125" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I125" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
@@ -4304,15 +4304,15 @@
         <v>3</v>
       </c>
       <c r="H126" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I126" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B127">
         <v>1</v>
@@ -4333,10 +4333,10 @@
         <v>3</v>
       </c>
       <c r="H127" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I127" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -4362,10 +4362,10 @@
         <v>4</v>
       </c>
       <c r="H128" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I128" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -4391,10 +4391,10 @@
         <v>4</v>
       </c>
       <c r="H129" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I129" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -4420,15 +4420,15 @@
         <v>4</v>
       </c>
       <c r="H130" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I130" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B131">
         <v>1</v>
@@ -4449,15 +4449,15 @@
         <v>6</v>
       </c>
       <c r="H131" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I131" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B132">
         <v>1</v>
@@ -4478,15 +4478,15 @@
         <v>6</v>
       </c>
       <c r="H132" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I132" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B133">
         <v>2</v>
@@ -4507,15 +4507,15 @@
         <v>6</v>
       </c>
       <c r="H133" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I133" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B134">
         <v>2</v>
@@ -4536,15 +4536,15 @@
         <v>7</v>
       </c>
       <c r="H134" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I134" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B135">
         <v>2</v>
@@ -4565,15 +4565,15 @@
         <v>7</v>
       </c>
       <c r="H135" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I135" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B136">
         <v>2</v>
@@ -4594,10 +4594,10 @@
         <v>4</v>
       </c>
       <c r="H136" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I136" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
@@ -4623,15 +4623,15 @@
         <v>5</v>
       </c>
       <c r="H137" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I137" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B138">
         <v>1</v>
@@ -4652,10 +4652,10 @@
         <v>5</v>
       </c>
       <c r="H138" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I138" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
@@ -4681,10 +4681,10 @@
         <v>6</v>
       </c>
       <c r="H139" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I139" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
@@ -4710,10 +4710,10 @@
         <v>6</v>
       </c>
       <c r="H140" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I140" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
@@ -4739,10 +4739,10 @@
         <v>5</v>
       </c>
       <c r="H141" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I141" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
@@ -4768,10 +4768,10 @@
         <v>5</v>
       </c>
       <c r="H142" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I142" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
@@ -4797,10 +4797,10 @@
         <v>5</v>
       </c>
       <c r="H143" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I143" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
@@ -4826,10 +4826,10 @@
         <v>6</v>
       </c>
       <c r="H144" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I144" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
@@ -4855,10 +4855,10 @@
         <v>6</v>
       </c>
       <c r="H145" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I145" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
@@ -4884,10 +4884,10 @@
         <v>6</v>
       </c>
       <c r="H146" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I146" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
@@ -4913,10 +4913,10 @@
         <v>7</v>
       </c>
       <c r="H147" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I147" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
@@ -4942,10 +4942,10 @@
         <v>7</v>
       </c>
       <c r="H148" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I148" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
@@ -4971,10 +4971,10 @@
         <v>8</v>
       </c>
       <c r="H149" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I149" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
@@ -5000,10 +5000,10 @@
         <v>7</v>
       </c>
       <c r="H150" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I150" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
@@ -5029,10 +5029,10 @@
         <v>7</v>
       </c>
       <c r="H151" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I151" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
@@ -5058,10 +5058,10 @@
         <v>1</v>
       </c>
       <c r="H152" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I152" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
@@ -5087,10 +5087,10 @@
         <v>2</v>
       </c>
       <c r="H153" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I153" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
@@ -5116,10 +5116,10 @@
         <v>2</v>
       </c>
       <c r="H154" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I154" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
@@ -5145,10 +5145,10 @@
         <v>4</v>
       </c>
       <c r="H155" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I155" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
@@ -5174,10 +5174,10 @@
         <v>4</v>
       </c>
       <c r="H156" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I156" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
@@ -5203,10 +5203,10 @@
         <v>5</v>
       </c>
       <c r="H157" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I157" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
@@ -5232,10 +5232,10 @@
         <v>5</v>
       </c>
       <c r="H158" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I158" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
@@ -5261,10 +5261,10 @@
         <v>9</v>
       </c>
       <c r="H159" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I159" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
@@ -5290,10 +5290,10 @@
         <v>7</v>
       </c>
       <c r="H160" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I160" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
@@ -5319,10 +5319,10 @@
         <v>7</v>
       </c>
       <c r="H161" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I161" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
@@ -5348,10 +5348,10 @@
         <v>8</v>
       </c>
       <c r="H162" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I162" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
@@ -5377,10 +5377,10 @@
         <v>8</v>
       </c>
       <c r="H163" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I163" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
@@ -5406,10 +5406,10 @@
         <v>3</v>
       </c>
       <c r="H164" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I164" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
@@ -5435,10 +5435,10 @@
         <v>3</v>
       </c>
       <c r="H165" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I165" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
@@ -5464,10 +5464,10 @@
         <v>6</v>
       </c>
       <c r="H166" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I166" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
@@ -5493,10 +5493,10 @@
         <v>6</v>
       </c>
       <c r="H167" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I167" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
@@ -5522,10 +5522,10 @@
         <v>6</v>
       </c>
       <c r="H168" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I168" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
@@ -5551,10 +5551,10 @@
         <v>9</v>
       </c>
       <c r="H169" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I169" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
@@ -5580,10 +5580,10 @@
         <v>9</v>
       </c>
       <c r="H170" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I170" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
@@ -5609,10 +5609,10 @@
         <v>8</v>
       </c>
       <c r="H171" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I171" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
@@ -5638,10 +5638,10 @@
         <v>8</v>
       </c>
       <c r="H172" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I172" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
@@ -5667,10 +5667,10 @@
         <v>7</v>
       </c>
       <c r="H173" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I173" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
@@ -5696,10 +5696,10 @@
         <v>7</v>
       </c>
       <c r="H174" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I174" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
@@ -5725,10 +5725,10 @@
         <v>7</v>
       </c>
       <c r="H175" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I175" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
@@ -5754,10 +5754,10 @@
         <v>7</v>
       </c>
       <c r="H176" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I176" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
@@ -5783,10 +5783,10 @@
         <v>8</v>
       </c>
       <c r="H177" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I177" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
@@ -5812,10 +5812,10 @@
         <v>8</v>
       </c>
       <c r="H178" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I178" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
@@ -5841,10 +5841,10 @@
         <v>9</v>
       </c>
       <c r="H179" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I179" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
@@ -5870,10 +5870,10 @@
         <v>10</v>
       </c>
       <c r="H180" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I180" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
@@ -5899,10 +5899,10 @@
         <v>8</v>
       </c>
       <c r="H181" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I181" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
@@ -5928,10 +5928,10 @@
         <v>1</v>
       </c>
       <c r="H182" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I182" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
@@ -5957,10 +5957,10 @@
         <v>2</v>
       </c>
       <c r="H183" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I183" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
@@ -5986,10 +5986,10 @@
         <v>2</v>
       </c>
       <c r="H184" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I184" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
@@ -6015,10 +6015,10 @@
         <v>4</v>
       </c>
       <c r="H185" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I185" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
@@ -6044,10 +6044,10 @@
         <v>4</v>
       </c>
       <c r="H186" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I186" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
@@ -6073,10 +6073,10 @@
         <v>5</v>
       </c>
       <c r="H187" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I187" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
@@ -6102,10 +6102,10 @@
         <v>5</v>
       </c>
       <c r="H188" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I188" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
@@ -6131,10 +6131,10 @@
         <v>5</v>
       </c>
       <c r="H189" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I189" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
@@ -6160,10 +6160,10 @@
         <v>9</v>
       </c>
       <c r="H190" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I190" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
@@ -6189,10 +6189,10 @@
         <v>7</v>
       </c>
       <c r="H191" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I191" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
@@ -6218,10 +6218,10 @@
         <v>7</v>
       </c>
       <c r="H192" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I192" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
@@ -6247,10 +6247,10 @@
         <v>8</v>
       </c>
       <c r="H193" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I193" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
@@ -6276,10 +6276,10 @@
         <v>8</v>
       </c>
       <c r="H194" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I194" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
@@ -6305,10 +6305,10 @@
         <v>3</v>
       </c>
       <c r="H195" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I195" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
@@ -6334,10 +6334,10 @@
         <v>3</v>
       </c>
       <c r="H196" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I196" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.25">
@@ -6363,10 +6363,10 @@
         <v>6</v>
       </c>
       <c r="H197" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I197" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.25">
@@ -6392,10 +6392,10 @@
         <v>6</v>
       </c>
       <c r="H198" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I198" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.25">
@@ -6421,10 +6421,10 @@
         <v>7</v>
       </c>
       <c r="H199" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I199" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
@@ -6450,10 +6450,10 @@
         <v>7</v>
       </c>
       <c r="H200" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I200" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
@@ -6479,10 +6479,10 @@
         <v>6</v>
       </c>
       <c r="H201" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I201" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.25">
@@ -6508,10 +6508,10 @@
         <v>6</v>
       </c>
       <c r="H202" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I202" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
@@ -6537,10 +6537,10 @@
         <v>7</v>
       </c>
       <c r="H203" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I203" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
@@ -6566,10 +6566,10 @@
         <v>8</v>
       </c>
       <c r="H204" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I204" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
@@ -6595,10 +6595,10 @@
         <v>8</v>
       </c>
       <c r="H205" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I205" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
@@ -6624,10 +6624,10 @@
         <v>8</v>
       </c>
       <c r="H206" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I206" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
@@ -6653,10 +6653,10 @@
         <v>9</v>
       </c>
       <c r="H207" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I207" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.25">
@@ -6682,10 +6682,10 @@
         <v>9</v>
       </c>
       <c r="H208" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I208" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
@@ -6711,10 +6711,10 @@
         <v>10</v>
       </c>
       <c r="H209" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I209" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
@@ -6740,10 +6740,10 @@
         <v>8</v>
       </c>
       <c r="H210" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I210" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
@@ -6769,10 +6769,10 @@
         <v>9</v>
       </c>
       <c r="H211" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I211" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
@@ -6795,10 +6795,10 @@
         <v>1</v>
       </c>
       <c r="H212" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I212" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
@@ -6821,10 +6821,10 @@
         <v>3</v>
       </c>
       <c r="H213" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I213" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
@@ -6847,10 +6847,10 @@
         <v>3</v>
       </c>
       <c r="H214" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I214" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
@@ -6873,10 +6873,10 @@
         <v>2</v>
       </c>
       <c r="H215" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I215" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
@@ -6899,10 +6899,10 @@
         <v>2</v>
       </c>
       <c r="H216" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I216" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
@@ -6925,10 +6925,10 @@
         <v>5</v>
       </c>
       <c r="H217" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I217" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.25">
@@ -6951,15 +6951,15 @@
         <v>5</v>
       </c>
       <c r="H218" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I218" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B219">
         <v>2</v>
@@ -6977,10 +6977,10 @@
         <v>7</v>
       </c>
       <c r="H219" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I219" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
@@ -7003,15 +7003,15 @@
         <v>6</v>
       </c>
       <c r="H220" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I220" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B221">
         <v>1</v>
@@ -7029,10 +7029,10 @@
         <v>6</v>
       </c>
       <c r="H221" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I221" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.25">
@@ -7055,10 +7055,10 @@
         <v>6</v>
       </c>
       <c r="H222" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I222" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.25">
@@ -7081,10 +7081,10 @@
         <v>6</v>
       </c>
       <c r="H223" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I223" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.25">
@@ -7107,10 +7107,10 @@
         <v>7</v>
       </c>
       <c r="H224" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I224" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.25">
@@ -7133,10 +7133,10 @@
         <v>4</v>
       </c>
       <c r="H225" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I225" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.25">
@@ -7159,10 +7159,10 @@
         <v>4</v>
       </c>
       <c r="H226" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I226" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.25">
@@ -7185,10 +7185,10 @@
         <v>7</v>
       </c>
       <c r="H227" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I227" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.25">
@@ -7211,10 +7211,10 @@
         <v>7</v>
       </c>
       <c r="H228" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I228" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.25">
@@ -7237,10 +7237,10 @@
         <v>7</v>
       </c>
       <c r="H229" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I229" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.25">
@@ -7263,10 +7263,10 @@
         <v>8</v>
       </c>
       <c r="H230" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I230" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.25">
@@ -7289,10 +7289,10 @@
         <v>8</v>
       </c>
       <c r="H231" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I231" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.25">
@@ -7315,10 +7315,10 @@
         <v>9</v>
       </c>
       <c r="H232" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I232" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
@@ -7341,10 +7341,10 @@
         <v>8</v>
       </c>
       <c r="H233" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="I233" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.25">
@@ -7370,7 +7370,7 @@
         <v>43</v>
       </c>
       <c r="I234" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.25">
@@ -7396,7 +7396,7 @@
         <v>43</v>
       </c>
       <c r="I235" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.25">
@@ -7422,7 +7422,7 @@
         <v>43</v>
       </c>
       <c r="I236" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.25">
@@ -7448,7 +7448,7 @@
         <v>43</v>
       </c>
       <c r="I237" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.25">
@@ -7474,7 +7474,7 @@
         <v>43</v>
       </c>
       <c r="I238" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.25">
@@ -7500,7 +7500,7 @@
         <v>43</v>
       </c>
       <c r="I239" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.25">
@@ -7526,7 +7526,7 @@
         <v>43</v>
       </c>
       <c r="I240" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.25">
@@ -7552,7 +7552,7 @@
         <v>43</v>
       </c>
       <c r="I241" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.25">
@@ -7578,7 +7578,7 @@
         <v>43</v>
       </c>
       <c r="I242" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.25">
@@ -7604,7 +7604,7 @@
         <v>43</v>
       </c>
       <c r="I243" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.25">
@@ -7630,7 +7630,7 @@
         <v>43</v>
       </c>
       <c r="I244" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.25">
@@ -7656,7 +7656,7 @@
         <v>43</v>
       </c>
       <c r="I245" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.25">
@@ -7682,7 +7682,7 @@
         <v>43</v>
       </c>
       <c r="I246" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.25">
@@ -7708,7 +7708,7 @@
         <v>43</v>
       </c>
       <c r="I247" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.25">
@@ -7734,7 +7734,7 @@
         <v>43</v>
       </c>
       <c r="I248" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.25">
@@ -7760,7 +7760,7 @@
         <v>43</v>
       </c>
       <c r="I249" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.25">
@@ -7786,7 +7786,7 @@
         <v>49</v>
       </c>
       <c r="I250" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.25">
@@ -7812,7 +7812,7 @@
         <v>49</v>
       </c>
       <c r="I251" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="252" spans="1:9" x14ac:dyDescent="0.25">
@@ -7838,7 +7838,7 @@
         <v>49</v>
       </c>
       <c r="I252" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="253" spans="1:9" x14ac:dyDescent="0.25">
@@ -7864,7 +7864,7 @@
         <v>49</v>
       </c>
       <c r="I253" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="254" spans="1:9" x14ac:dyDescent="0.25">
@@ -7890,7 +7890,7 @@
         <v>49</v>
       </c>
       <c r="I254" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="255" spans="1:9" x14ac:dyDescent="0.25">
@@ -7916,7 +7916,7 @@
         <v>49</v>
       </c>
       <c r="I255" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.25">
@@ -7942,7 +7942,7 @@
         <v>49</v>
       </c>
       <c r="I256" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="257" spans="1:9" x14ac:dyDescent="0.25">
@@ -7968,7 +7968,7 @@
         <v>49</v>
       </c>
       <c r="I257" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="258" spans="1:9" x14ac:dyDescent="0.25">
@@ -7994,7 +7994,7 @@
         <v>49</v>
       </c>
       <c r="I258" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="259" spans="1:9" x14ac:dyDescent="0.25">
@@ -8020,7 +8020,7 @@
         <v>49</v>
       </c>
       <c r="I259" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="260" spans="1:9" x14ac:dyDescent="0.25">
@@ -8046,7 +8046,7 @@
         <v>49</v>
       </c>
       <c r="I260" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="261" spans="1:9" x14ac:dyDescent="0.25">
@@ -8072,7 +8072,7 @@
         <v>49</v>
       </c>
       <c r="I261" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="262" spans="1:9" x14ac:dyDescent="0.25">
@@ -8098,7 +8098,7 @@
         <v>49</v>
       </c>
       <c r="I262" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="263" spans="1:9" x14ac:dyDescent="0.25">
@@ -8124,7 +8124,7 @@
         <v>49</v>
       </c>
       <c r="I263" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="264" spans="1:9" x14ac:dyDescent="0.25">
@@ -8150,7 +8150,7 @@
         <v>49</v>
       </c>
       <c r="I264" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="265" spans="1:9" x14ac:dyDescent="0.25">
@@ -8176,7 +8176,7 @@
         <v>49</v>
       </c>
       <c r="I265" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="266" spans="1:9" x14ac:dyDescent="0.25">
@@ -8202,7 +8202,7 @@
         <v>49</v>
       </c>
       <c r="I266" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="267" spans="1:9" x14ac:dyDescent="0.25">
@@ -8228,7 +8228,7 @@
         <v>49</v>
       </c>
       <c r="I267" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="268" spans="1:9" x14ac:dyDescent="0.25">
@@ -8251,10 +8251,10 @@
         <v>1</v>
       </c>
       <c r="H268" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I268" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="269" spans="1:9" x14ac:dyDescent="0.25">
@@ -8277,10 +8277,10 @@
         <v>2</v>
       </c>
       <c r="H269" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I269" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="270" spans="1:9" x14ac:dyDescent="0.25">
@@ -8303,10 +8303,10 @@
         <v>2</v>
       </c>
       <c r="H270" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I270" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.25">
@@ -8329,15 +8329,15 @@
         <v>3</v>
       </c>
       <c r="H271" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I271" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B272">
         <v>1</v>
@@ -8355,10 +8355,10 @@
         <v>3</v>
       </c>
       <c r="H272" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I272" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="273" spans="1:9" x14ac:dyDescent="0.25">
@@ -8381,10 +8381,10 @@
         <v>9</v>
       </c>
       <c r="H273" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I273" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.25">
@@ -8407,10 +8407,10 @@
         <v>7</v>
       </c>
       <c r="H274" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I274" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="275" spans="1:9" x14ac:dyDescent="0.25">
@@ -8433,15 +8433,15 @@
         <v>7</v>
       </c>
       <c r="H275" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I275" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B276">
         <v>2</v>
@@ -8459,10 +8459,10 @@
         <v>7</v>
       </c>
       <c r="H276" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I276" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.25">
@@ -8485,10 +8485,10 @@
         <v>8</v>
       </c>
       <c r="H277" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I277" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.25">
@@ -8511,15 +8511,15 @@
         <v>8</v>
       </c>
       <c r="H278" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I278" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B279">
         <v>1</v>
@@ -8537,15 +8537,15 @@
         <v>8</v>
       </c>
       <c r="H279" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I279" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B280">
         <v>1</v>
@@ -8563,15 +8563,15 @@
         <v>8</v>
       </c>
       <c r="H280" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I280" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B281">
         <v>2</v>
@@ -8589,15 +8589,15 @@
         <v>4</v>
       </c>
       <c r="H281" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I281" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="282" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B282">
         <v>1</v>
@@ -8615,10 +8615,10 @@
         <v>4</v>
       </c>
       <c r="H282" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I282" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="283" spans="1:9" x14ac:dyDescent="0.25">
@@ -8641,15 +8641,15 @@
         <v>8</v>
       </c>
       <c r="H283" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I283" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="284" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B284">
         <v>2</v>
@@ -8667,15 +8667,15 @@
         <v>5</v>
       </c>
       <c r="H284" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I284" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="285" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B285">
         <v>1</v>
@@ -8693,15 +8693,15 @@
         <v>5</v>
       </c>
       <c r="H285" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I285" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="286" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B286">
         <v>2</v>
@@ -8719,15 +8719,15 @@
         <v>6</v>
       </c>
       <c r="H286" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I286" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="287" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B287">
         <v>1</v>
@@ -8745,15 +8745,15 @@
         <v>6</v>
       </c>
       <c r="H287" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I287" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="288" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B288">
         <v>2</v>
@@ -8771,15 +8771,15 @@
         <v>9</v>
       </c>
       <c r="H288" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I288" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="289" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B289">
         <v>1</v>
@@ -8797,15 +8797,15 @@
         <v>9</v>
       </c>
       <c r="H289" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I289" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="290" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B290">
         <v>2</v>
@@ -8823,15 +8823,15 @@
         <v>9</v>
       </c>
       <c r="H290" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I290" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B291">
         <v>2</v>
@@ -8849,10 +8849,10 @@
         <v>10</v>
       </c>
       <c r="H291" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I291" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>